<commit_message>
Update report-checklist.xlsx according to feedback.
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111#ALFADOCSITALIASRLXX/AlfaDocs_Italia_srl/AlfaDocs/20240717/report-checklist.xlsx
+++ b/GATEWAY/A1#111#ALFADOCSITALIASRLXX/AlfaDocs_Italia_srl/AlfaDocs/20240717/report-checklist.xlsx
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="509" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="489" uniqueCount="208">
   <si>
     <t xml:space="preserve">COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -344,9 +344,6 @@
     <t xml:space="preserve">Campo valorizzato di default</t>
   </si>
   <si>
-    <t xml:space="preserve">Il token JWT viene generato programmaticamente e come default usiamo sempre il valore ‘TREATMENT’ per la validazione.</t>
-  </si>
-  <si>
     <t xml:space="preserve">KO</t>
   </si>
   <si>
@@ -409,9 +406,6 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Il token JWT viene generato programmaticamente e come default usiamo sempre il action_Id ‘CREATE’ per la validazione.</t>
-  </si>
-  <si>
     <t xml:space="preserve">VALIDAZIONE_TOKEN_JWT_CAMPO_RSA_KO</t>
   </si>
   <si>
@@ -453,9 +447,6 @@
     <t xml:space="preserve">L’applicativo effettua controlli preventivi sul dato inserito</t>
   </si>
   <si>
-    <t xml:space="preserve">L'applicativo sempre richiede di impostare il livello di riservatezza</t>
-  </si>
-  <si>
     <t xml:space="preserve">VALIDAZIONE_CDA2_RAD_CT6_KO</t>
   </si>
   <si>
@@ -479,9 +470,6 @@
     <t xml:space="preserve">Campo valorizzabile tramite selezione da un set di valori ammessi</t>
   </si>
   <si>
-    <t xml:space="preserve">L'applicativo non consente la registrazione di un livello di riservatezza diverso da Normale e Very Restricted</t>
-  </si>
-  <si>
     <t xml:space="preserve">VALIDAZIONE_CDA2_RAD_CT8_KO</t>
   </si>
   <si>
@@ -492,9 +480,6 @@
     <t xml:space="preserve">Campo/sezione non gestito/a in modo strutturato dall’applicativo</t>
   </si>
   <si>
-    <t xml:space="preserve">L’applicativo non gestisce l’indirizzo dell’assistito (Indirizzo del paziente &lt;addr&gt;)</t>
-  </si>
-  <si>
     <t xml:space="preserve">VALIDAZIONE_CDA2_RAD_CT9_KO</t>
   </si>
   <si>
@@ -502,9 +487,6 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 9" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t xml:space="preserve">L'applicazione richiede il nome e il cognome del paziente prima di creare un Referto.</t>
-  </si>
-  <si>
     <t xml:space="preserve">VALIDAZIONE_CDA2_RAD_CT10_KO</t>
   </si>
   <si>
@@ -536,9 +518,6 @@
     <t xml:space="preserve">Campo obbligatorio</t>
   </si>
   <si>
-    <t xml:space="preserve">Se l'utente specifica che esiste una prescrizione, il sistema si assicura che venga fornito un numero di identificazione della prescrizione. </t>
-  </si>
-  <si>
     <t xml:space="preserve">VALIDAZIONE_CDA2_RAD_CT14_KO</t>
   </si>
   <si>
@@ -546,17 +525,11 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 14" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t xml:space="preserve">L'applicazione assicura che l'utente specifichi sempre le informazioni per l'esame eseguito (act/code).</t>
-  </si>
-  <si>
     <t xml:space="preserve">VALIDAZIONE_CDA2_RAD_CT15_KO</t>
   </si>
   <si>
     <t xml:space="preserve">Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori semantici sui Dati (status code 422), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 15" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">L'applicazione assicura che l'utente specifichi sempre il Referto.</t>
   </si>
   <si>
     <t xml:space="preserve">VALIDAZIONE_CDA2_RAD_CT16_KO</t>
@@ -624,9 +597,6 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">Elementi opzionali non gestiti</t>
-  </si>
-  <si>
     <t xml:space="preserve">OK</t>
   </si>
   <si>
@@ -722,9 +692,6 @@
   <si>
     <t xml:space="preserve">Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori sintattici sui Dati (status code 400), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 14" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">L'applicazione assicura che l'utente specifichi sempre le informazioni per le prestazioni (act/code).</t>
   </si>
   <si>
     <t xml:space="preserve">VALIDAZIONE_CDA2_RSA_CT15_KO</t>
@@ -1656,11 +1623,11 @@
   </sheetPr>
   <dimension ref="A1:A13"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="39" zoomScaleNormal="39" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.46484375" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.47265625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="130.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="2" style="0" width="8.82"/>
@@ -1743,11 +1710,11 @@
   </sheetPr>
   <dimension ref="A1:B996"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="39" zoomScaleNormal="39" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.46484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.47265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="194.18"/>
@@ -2820,15 +2787,15 @@
   </sheetPr>
   <dimension ref="A1:W1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="39" zoomScaleNormal="39" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="9" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="J14" activeCellId="0" sqref="J14"/>
+      <selection pane="bottomRight" activeCell="L52" activeCellId="0" sqref="L52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.46484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.47265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="46.83"/>
@@ -3138,9 +3105,7 @@
       <c r="K10" s="31" t="s">
         <v>52</v>
       </c>
-      <c r="L10" s="31" t="s">
-        <v>53</v>
-      </c>
+      <c r="L10" s="31"/>
       <c r="M10" s="31"/>
       <c r="N10" s="31"/>
       <c r="O10" s="31"/>
@@ -3152,7 +3117,7 @@
       <c r="U10" s="32"/>
       <c r="V10" s="33"/>
       <c r="W10" s="34" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="135.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3163,10 +3128,10 @@
         <v>47</v>
       </c>
       <c r="C11" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="D11" s="27" t="s">
         <v>55</v>
-      </c>
-      <c r="D11" s="27" t="s">
-        <v>56</v>
       </c>
       <c r="E11" s="28" t="s">
         <v>50</v>
@@ -3181,9 +3146,7 @@
       <c r="K11" s="31" t="s">
         <v>52</v>
       </c>
-      <c r="L11" s="31" t="s">
-        <v>53</v>
-      </c>
+      <c r="L11" s="31"/>
       <c r="M11" s="31"/>
       <c r="N11" s="31"/>
       <c r="O11" s="31"/>
@@ -3195,7 +3158,7 @@
       <c r="U11" s="32"/>
       <c r="V11" s="33"/>
       <c r="W11" s="34" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="164.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3209,10 +3172,10 @@
         <v>48</v>
       </c>
       <c r="D12" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="E12" s="28" t="s">
         <v>57</v>
-      </c>
-      <c r="E12" s="28" t="s">
-        <v>58</v>
       </c>
       <c r="F12" s="29"/>
       <c r="G12" s="30"/>
@@ -3224,9 +3187,7 @@
       <c r="K12" s="31" t="s">
         <v>52</v>
       </c>
-      <c r="L12" s="31" t="s">
-        <v>59</v>
-      </c>
+      <c r="L12" s="31"/>
       <c r="M12" s="31"/>
       <c r="N12" s="31"/>
       <c r="O12" s="31"/>
@@ -3238,7 +3199,7 @@
       <c r="U12" s="32"/>
       <c r="V12" s="33"/>
       <c r="W12" s="34" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="129.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3249,13 +3210,13 @@
         <v>47</v>
       </c>
       <c r="C13" s="27" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D13" s="27" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E13" s="28" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F13" s="29"/>
       <c r="G13" s="30"/>
@@ -3267,9 +3228,7 @@
       <c r="K13" s="31" t="s">
         <v>52</v>
       </c>
-      <c r="L13" s="31" t="s">
-        <v>59</v>
-      </c>
+      <c r="L13" s="31"/>
       <c r="M13" s="31"/>
       <c r="N13" s="31"/>
       <c r="O13" s="31"/>
@@ -3281,7 +3240,7 @@
       <c r="U13" s="32"/>
       <c r="V13" s="33"/>
       <c r="W13" s="34" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="116.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3295,21 +3254,21 @@
         <v>48</v>
       </c>
       <c r="D14" s="27" t="s">
+        <v>59</v>
+      </c>
+      <c r="E14" s="35" t="s">
+        <v>60</v>
+      </c>
+      <c r="F14" s="29" t="s">
         <v>61</v>
       </c>
-      <c r="E14" s="35" t="s">
+      <c r="G14" s="30" t="s">
         <v>62</v>
-      </c>
-      <c r="F14" s="29" t="s">
-        <v>63</v>
-      </c>
-      <c r="G14" s="30" t="s">
-        <v>64</v>
       </c>
       <c r="H14" s="30"/>
       <c r="I14" s="30"/>
       <c r="J14" s="31" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="K14" s="31"/>
       <c r="L14" s="31"/>
@@ -3317,30 +3276,30 @@
         <v>51</v>
       </c>
       <c r="N14" s="31" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="O14" s="31" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="P14" s="31" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="Q14" s="31" t="s">
         <v>51</v>
       </c>
       <c r="R14" s="31" t="s">
+        <v>63</v>
+      </c>
+      <c r="S14" s="31" t="s">
         <v>65</v>
-      </c>
-      <c r="S14" s="31" t="s">
-        <v>67</v>
       </c>
       <c r="T14" s="31"/>
       <c r="U14" s="32" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="V14" s="33"/>
       <c r="W14" s="34" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="153.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3351,24 +3310,24 @@
         <v>47</v>
       </c>
       <c r="C15" s="27" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D15" s="27" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E15" s="35" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F15" s="29" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="G15" s="30" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="H15" s="30"/>
       <c r="I15" s="30"/>
       <c r="J15" s="31" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="K15" s="31"/>
       <c r="L15" s="31"/>
@@ -3376,30 +3335,30 @@
         <v>51</v>
       </c>
       <c r="N15" s="31" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="O15" s="31" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="P15" s="31" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="Q15" s="31" t="s">
         <v>51</v>
       </c>
       <c r="R15" s="31" t="s">
+        <v>63</v>
+      </c>
+      <c r="S15" s="31" t="s">
         <v>65</v>
-      </c>
-      <c r="S15" s="31" t="s">
-        <v>67</v>
       </c>
       <c r="T15" s="31"/>
       <c r="U15" s="32" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="V15" s="33"/>
       <c r="W15" s="34" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="138.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3413,10 +3372,10 @@
         <v>48</v>
       </c>
       <c r="D16" s="27" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E16" s="35" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F16" s="29"/>
       <c r="G16" s="30"/>
@@ -3426,11 +3385,9 @@
         <v>51</v>
       </c>
       <c r="K16" s="31" t="s">
-        <v>72</v>
-      </c>
-      <c r="L16" s="31" t="s">
-        <v>73</v>
-      </c>
+        <v>70</v>
+      </c>
+      <c r="L16" s="31"/>
       <c r="M16" s="31"/>
       <c r="N16" s="31"/>
       <c r="O16" s="31"/>
@@ -3442,7 +3399,7 @@
       <c r="U16" s="32"/>
       <c r="V16" s="33"/>
       <c r="W16" s="34" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="126" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3456,10 +3413,10 @@
         <v>48</v>
       </c>
       <c r="D17" s="27" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="E17" s="35" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="F17" s="29"/>
       <c r="G17" s="30"/>
@@ -3469,10 +3426,10 @@
         <v>51</v>
       </c>
       <c r="K17" s="31" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="L17" s="31" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="M17" s="31"/>
       <c r="N17" s="31"/>
@@ -3485,7 +3442,7 @@
       <c r="U17" s="32"/>
       <c r="V17" s="33"/>
       <c r="W17" s="34" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="119.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3499,10 +3456,10 @@
         <v>48</v>
       </c>
       <c r="D18" s="27" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="E18" s="35" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="F18" s="29"/>
       <c r="G18" s="30"/>
@@ -3512,11 +3469,9 @@
         <v>51</v>
       </c>
       <c r="K18" s="31" t="s">
-        <v>80</v>
-      </c>
-      <c r="L18" s="31" t="s">
-        <v>81</v>
-      </c>
+        <v>77</v>
+      </c>
+      <c r="L18" s="31"/>
       <c r="M18" s="31"/>
       <c r="N18" s="31"/>
       <c r="O18" s="31"/>
@@ -3528,7 +3483,7 @@
       <c r="U18" s="32"/>
       <c r="V18" s="33"/>
       <c r="W18" s="34" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="131" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3542,10 +3497,10 @@
         <v>48</v>
       </c>
       <c r="D19" s="27" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="E19" s="35" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="F19" s="29"/>
       <c r="G19" s="30"/>
@@ -3555,11 +3510,9 @@
         <v>51</v>
       </c>
       <c r="K19" s="31" t="s">
-        <v>84</v>
-      </c>
-      <c r="L19" s="31" t="s">
-        <v>85</v>
-      </c>
+        <v>80</v>
+      </c>
+      <c r="L19" s="31"/>
       <c r="M19" s="31"/>
       <c r="N19" s="31"/>
       <c r="O19" s="31"/>
@@ -3571,7 +3524,7 @@
       <c r="U19" s="32"/>
       <c r="V19" s="33"/>
       <c r="W19" s="34" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="108.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3585,10 +3538,10 @@
         <v>48</v>
       </c>
       <c r="D20" s="27" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="E20" s="35" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="F20" s="29"/>
       <c r="G20" s="30"/>
@@ -3598,11 +3551,9 @@
         <v>51</v>
       </c>
       <c r="K20" s="31" t="s">
-        <v>72</v>
-      </c>
-      <c r="L20" s="31" t="s">
-        <v>88</v>
-      </c>
+        <v>70</v>
+      </c>
+      <c r="L20" s="31"/>
       <c r="M20" s="31"/>
       <c r="N20" s="31"/>
       <c r="O20" s="31"/>
@@ -3614,7 +3565,7 @@
       <c r="U20" s="32"/>
       <c r="V20" s="33"/>
       <c r="W20" s="34" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="108.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3628,10 +3579,10 @@
         <v>48</v>
       </c>
       <c r="D21" s="27" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="E21" s="35" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="F21" s="29"/>
       <c r="G21" s="30"/>
@@ -3641,7 +3592,7 @@
         <v>51</v>
       </c>
       <c r="K21" s="31" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="L21" s="31"/>
       <c r="M21" s="31"/>
@@ -3655,7 +3606,7 @@
       <c r="U21" s="32"/>
       <c r="V21" s="33"/>
       <c r="W21" s="34" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="93.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3669,10 +3620,10 @@
         <v>48</v>
       </c>
       <c r="D22" s="27" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="E22" s="35" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="F22" s="29"/>
       <c r="G22" s="30"/>
@@ -3682,7 +3633,7 @@
         <v>51</v>
       </c>
       <c r="K22" s="31" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="L22" s="31"/>
       <c r="M22" s="31"/>
@@ -3696,7 +3647,7 @@
       <c r="U22" s="32"/>
       <c r="V22" s="33"/>
       <c r="W22" s="34" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="104.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3710,10 +3661,10 @@
         <v>48</v>
       </c>
       <c r="D23" s="27" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="E23" s="35" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="F23" s="29"/>
       <c r="G23" s="30"/>
@@ -3723,7 +3674,7 @@
         <v>51</v>
       </c>
       <c r="K23" s="31" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="L23" s="31"/>
       <c r="M23" s="31"/>
@@ -3737,7 +3688,7 @@
       <c r="U23" s="32"/>
       <c r="V23" s="33"/>
       <c r="W23" s="34" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="90.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3751,10 +3702,10 @@
         <v>48</v>
       </c>
       <c r="D24" s="27" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="E24" s="35" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="F24" s="29"/>
       <c r="G24" s="30"/>
@@ -3764,11 +3715,9 @@
         <v>51</v>
       </c>
       <c r="K24" s="31" t="s">
-        <v>97</v>
-      </c>
-      <c r="L24" s="31" t="s">
-        <v>98</v>
-      </c>
+        <v>91</v>
+      </c>
+      <c r="L24" s="31"/>
       <c r="M24" s="31"/>
       <c r="N24" s="31"/>
       <c r="O24" s="31"/>
@@ -3780,7 +3729,7 @@
       <c r="U24" s="32"/>
       <c r="V24" s="33"/>
       <c r="W24" s="34" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="93.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3794,10 +3743,10 @@
         <v>48</v>
       </c>
       <c r="D25" s="27" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="E25" s="35" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="F25" s="29"/>
       <c r="G25" s="30"/>
@@ -3807,11 +3756,9 @@
         <v>51</v>
       </c>
       <c r="K25" s="31" t="s">
-        <v>97</v>
-      </c>
-      <c r="L25" s="31" t="s">
-        <v>101</v>
-      </c>
+        <v>91</v>
+      </c>
+      <c r="L25" s="31"/>
       <c r="M25" s="31"/>
       <c r="N25" s="31"/>
       <c r="O25" s="31"/>
@@ -3823,7 +3770,7 @@
       <c r="U25" s="32"/>
       <c r="V25" s="33"/>
       <c r="W25" s="34" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="92.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3837,10 +3784,10 @@
         <v>48</v>
       </c>
       <c r="D26" s="27" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="E26" s="35" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="F26" s="29"/>
       <c r="G26" s="30"/>
@@ -3850,11 +3797,9 @@
         <v>51</v>
       </c>
       <c r="K26" s="31" t="s">
-        <v>97</v>
-      </c>
-      <c r="L26" s="31" t="s">
-        <v>104</v>
-      </c>
+        <v>91</v>
+      </c>
+      <c r="L26" s="31"/>
       <c r="M26" s="31"/>
       <c r="N26" s="31"/>
       <c r="O26" s="31"/>
@@ -3866,7 +3811,7 @@
       <c r="U26" s="32"/>
       <c r="V26" s="33"/>
       <c r="W26" s="34" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="98.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3880,10 +3825,10 @@
         <v>48</v>
       </c>
       <c r="D27" s="27" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="E27" s="35" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="F27" s="29"/>
       <c r="G27" s="30"/>
@@ -3893,7 +3838,7 @@
         <v>51</v>
       </c>
       <c r="K27" s="31" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="L27" s="31"/>
       <c r="M27" s="31"/>
@@ -3907,7 +3852,7 @@
       <c r="U27" s="32"/>
       <c r="V27" s="33"/>
       <c r="W27" s="34" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="89.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3921,10 +3866,10 @@
         <v>48</v>
       </c>
       <c r="D28" s="27" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="E28" s="35" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="F28" s="29"/>
       <c r="G28" s="30"/>
@@ -3934,7 +3879,7 @@
         <v>51</v>
       </c>
       <c r="K28" s="31" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="L28" s="31"/>
       <c r="M28" s="31"/>
@@ -3948,7 +3893,7 @@
       <c r="U28" s="32"/>
       <c r="V28" s="33"/>
       <c r="W28" s="34" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="95.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3962,10 +3907,10 @@
         <v>48</v>
       </c>
       <c r="D29" s="27" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="E29" s="35" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="F29" s="29"/>
       <c r="G29" s="30"/>
@@ -3975,7 +3920,7 @@
         <v>51</v>
       </c>
       <c r="K29" s="31" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="L29" s="31"/>
       <c r="M29" s="31"/>
@@ -3989,7 +3934,7 @@
       <c r="U29" s="32"/>
       <c r="V29" s="33"/>
       <c r="W29" s="34" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="94.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4003,10 +3948,10 @@
         <v>48</v>
       </c>
       <c r="D30" s="27" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="E30" s="35" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="F30" s="29"/>
       <c r="G30" s="30"/>
@@ -4016,7 +3961,7 @@
         <v>51</v>
       </c>
       <c r="K30" s="31" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="L30" s="31"/>
       <c r="M30" s="31"/>
@@ -4030,7 +3975,7 @@
       <c r="U30" s="32"/>
       <c r="V30" s="33"/>
       <c r="W30" s="34" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="91.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4044,10 +3989,10 @@
         <v>48</v>
       </c>
       <c r="D31" s="27" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="E31" s="35" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="F31" s="29"/>
       <c r="G31" s="30"/>
@@ -4057,7 +4002,7 @@
         <v>51</v>
       </c>
       <c r="K31" s="31" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="L31" s="31"/>
       <c r="M31" s="31"/>
@@ -4071,7 +4016,7 @@
       <c r="U31" s="32"/>
       <c r="V31" s="33"/>
       <c r="W31" s="34" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="91.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4085,10 +4030,10 @@
         <v>48</v>
       </c>
       <c r="D32" s="27" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="E32" s="35" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="F32" s="29"/>
       <c r="G32" s="30"/>
@@ -4098,7 +4043,7 @@
         <v>51</v>
       </c>
       <c r="K32" s="31" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="L32" s="31"/>
       <c r="M32" s="31"/>
@@ -4112,7 +4057,7 @@
       <c r="U32" s="32"/>
       <c r="V32" s="33"/>
       <c r="W32" s="34" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="89.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4126,10 +4071,10 @@
         <v>48</v>
       </c>
       <c r="D33" s="27" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="E33" s="35" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="F33" s="29"/>
       <c r="G33" s="30"/>
@@ -4139,7 +4084,7 @@
         <v>51</v>
       </c>
       <c r="K33" s="31" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="L33" s="31"/>
       <c r="M33" s="31"/>
@@ -4153,7 +4098,7 @@
       <c r="U33" s="32"/>
       <c r="V33" s="33"/>
       <c r="W33" s="34" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="101.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4167,10 +4112,10 @@
         <v>48</v>
       </c>
       <c r="D34" s="27" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="E34" s="35" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="F34" s="29"/>
       <c r="G34" s="30"/>
@@ -4180,7 +4125,7 @@
         <v>51</v>
       </c>
       <c r="K34" s="31" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="L34" s="31"/>
       <c r="M34" s="31"/>
@@ -4194,7 +4139,7 @@
       <c r="U34" s="32"/>
       <c r="V34" s="33"/>
       <c r="W34" s="34" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="120.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4205,13 +4150,13 @@
         <v>47</v>
       </c>
       <c r="C35" s="27" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D35" s="27" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="E35" s="35" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="F35" s="29"/>
       <c r="G35" s="30"/>
@@ -4221,11 +4166,9 @@
         <v>51</v>
       </c>
       <c r="K35" s="31" t="s">
-        <v>84</v>
-      </c>
-      <c r="L35" s="31" t="s">
-        <v>123</v>
-      </c>
+        <v>80</v>
+      </c>
+      <c r="L35" s="31"/>
       <c r="M35" s="31"/>
       <c r="N35" s="31"/>
       <c r="O35" s="31"/>
@@ -4237,7 +4180,7 @@
       <c r="U35" s="32"/>
       <c r="V35" s="33"/>
       <c r="W35" s="34" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="128.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4248,13 +4191,13 @@
         <v>47</v>
       </c>
       <c r="C36" s="27" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D36" s="27" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
       <c r="E36" s="35" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="F36" s="29"/>
       <c r="G36" s="30"/>
@@ -4264,7 +4207,7 @@
         <v>51</v>
       </c>
       <c r="K36" s="31" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="L36" s="31"/>
       <c r="M36" s="31"/>
@@ -4278,7 +4221,7 @@
       <c r="U36" s="32"/>
       <c r="V36" s="33"/>
       <c r="W36" s="34" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="118.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4289,13 +4232,13 @@
         <v>47</v>
       </c>
       <c r="C37" s="27" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D37" s="27" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="E37" s="35" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="F37" s="29"/>
       <c r="G37" s="30"/>
@@ -4305,7 +4248,7 @@
         <v>51</v>
       </c>
       <c r="K37" s="31" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="L37" s="31"/>
       <c r="M37" s="31"/>
@@ -4319,7 +4262,7 @@
       <c r="U37" s="32"/>
       <c r="V37" s="33"/>
       <c r="W37" s="34" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="129.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4330,13 +4273,13 @@
         <v>47</v>
       </c>
       <c r="C38" s="27" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D38" s="27" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="E38" s="35" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="F38" s="29"/>
       <c r="G38" s="30"/>
@@ -4346,7 +4289,7 @@
         <v>51</v>
       </c>
       <c r="K38" s="31" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="L38" s="31"/>
       <c r="M38" s="31"/>
@@ -4360,7 +4303,7 @@
       <c r="U38" s="32"/>
       <c r="V38" s="33"/>
       <c r="W38" s="34" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="102.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4371,13 +4314,13 @@
         <v>47</v>
       </c>
       <c r="C39" s="27" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D39" s="27" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="E39" s="35" t="s">
-        <v>132</v>
+        <v>122</v>
       </c>
       <c r="F39" s="29"/>
       <c r="G39" s="30"/>
@@ -4387,11 +4330,9 @@
         <v>51</v>
       </c>
       <c r="K39" s="31" t="s">
-        <v>72</v>
-      </c>
-      <c r="L39" s="31" t="s">
-        <v>73</v>
-      </c>
+        <v>70</v>
+      </c>
+      <c r="L39" s="31"/>
       <c r="M39" s="31"/>
       <c r="N39" s="31"/>
       <c r="O39" s="31"/>
@@ -4403,7 +4344,7 @@
       <c r="U39" s="32"/>
       <c r="V39" s="33"/>
       <c r="W39" s="34" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="103.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4414,13 +4355,13 @@
         <v>47</v>
       </c>
       <c r="C40" s="27" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D40" s="27" t="s">
-        <v>133</v>
+        <v>123</v>
       </c>
       <c r="E40" s="35" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
       <c r="F40" s="29"/>
       <c r="G40" s="30"/>
@@ -4430,10 +4371,10 @@
         <v>51</v>
       </c>
       <c r="K40" s="31" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="L40" s="31" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="M40" s="31"/>
       <c r="N40" s="31"/>
@@ -4446,7 +4387,7 @@
       <c r="U40" s="32"/>
       <c r="V40" s="33"/>
       <c r="W40" s="34" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="121.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4457,13 +4398,13 @@
         <v>47</v>
       </c>
       <c r="C41" s="27" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D41" s="27" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="E41" s="35" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
       <c r="F41" s="29"/>
       <c r="G41" s="30"/>
@@ -4473,11 +4414,9 @@
         <v>51</v>
       </c>
       <c r="K41" s="31" t="s">
-        <v>80</v>
-      </c>
-      <c r="L41" s="31" t="s">
-        <v>81</v>
-      </c>
+        <v>77</v>
+      </c>
+      <c r="L41" s="31"/>
       <c r="M41" s="31"/>
       <c r="N41" s="31"/>
       <c r="O41" s="31"/>
@@ -4489,7 +4428,7 @@
       <c r="U41" s="32"/>
       <c r="V41" s="33"/>
       <c r="W41" s="34" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="99.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4500,13 +4439,13 @@
         <v>47</v>
       </c>
       <c r="C42" s="27" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D42" s="27" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
       <c r="E42" s="35" t="s">
-        <v>138</v>
+        <v>128</v>
       </c>
       <c r="F42" s="29"/>
       <c r="G42" s="30"/>
@@ -4516,11 +4455,9 @@
         <v>51</v>
       </c>
       <c r="K42" s="31" t="s">
-        <v>84</v>
-      </c>
-      <c r="L42" s="31" t="s">
-        <v>85</v>
-      </c>
+        <v>80</v>
+      </c>
+      <c r="L42" s="31"/>
       <c r="M42" s="31"/>
       <c r="N42" s="31"/>
       <c r="O42" s="31"/>
@@ -4532,7 +4469,7 @@
       <c r="U42" s="32"/>
       <c r="V42" s="33"/>
       <c r="W42" s="34" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="141.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4543,13 +4480,13 @@
         <v>47</v>
       </c>
       <c r="C43" s="27" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D43" s="27" t="s">
-        <v>139</v>
+        <v>129</v>
       </c>
       <c r="E43" s="35" t="s">
-        <v>140</v>
+        <v>130</v>
       </c>
       <c r="F43" s="29"/>
       <c r="G43" s="30"/>
@@ -4559,11 +4496,9 @@
         <v>51</v>
       </c>
       <c r="K43" s="31" t="s">
-        <v>72</v>
-      </c>
-      <c r="L43" s="31" t="s">
-        <v>88</v>
-      </c>
+        <v>70</v>
+      </c>
+      <c r="L43" s="31"/>
       <c r="M43" s="31"/>
       <c r="N43" s="31"/>
       <c r="O43" s="31"/>
@@ -4575,7 +4510,7 @@
       <c r="U43" s="32"/>
       <c r="V43" s="33"/>
       <c r="W43" s="34" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="110.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4586,13 +4521,13 @@
         <v>47</v>
       </c>
       <c r="C44" s="27" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D44" s="27" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
       <c r="E44" s="35" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="F44" s="29"/>
       <c r="G44" s="30"/>
@@ -4602,7 +4537,7 @@
         <v>51</v>
       </c>
       <c r="K44" s="31" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="L44" s="31"/>
       <c r="M44" s="31"/>
@@ -4616,7 +4551,7 @@
       <c r="U44" s="32"/>
       <c r="V44" s="33"/>
       <c r="W44" s="34" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="144.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4627,13 +4562,13 @@
         <v>47</v>
       </c>
       <c r="C45" s="27" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D45" s="27" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="E45" s="35" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="F45" s="29"/>
       <c r="G45" s="30"/>
@@ -4643,7 +4578,7 @@
         <v>51</v>
       </c>
       <c r="K45" s="31" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="L45" s="31"/>
       <c r="M45" s="31"/>
@@ -4657,7 +4592,7 @@
       <c r="U45" s="32"/>
       <c r="V45" s="33"/>
       <c r="W45" s="34" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="115.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4668,13 +4603,13 @@
         <v>47</v>
       </c>
       <c r="C46" s="27" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D46" s="27" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
       <c r="E46" s="35" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
       <c r="F46" s="29"/>
       <c r="G46" s="30"/>
@@ -4684,7 +4619,7 @@
         <v>51</v>
       </c>
       <c r="K46" s="31" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="L46" s="31"/>
       <c r="M46" s="31"/>
@@ -4698,7 +4633,7 @@
       <c r="U46" s="32"/>
       <c r="V46" s="33"/>
       <c r="W46" s="34" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="140.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4709,13 +4644,13 @@
         <v>47</v>
       </c>
       <c r="C47" s="27" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D47" s="27" t="s">
-        <v>147</v>
+        <v>137</v>
       </c>
       <c r="E47" s="35" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
       <c r="F47" s="29"/>
       <c r="G47" s="30"/>
@@ -4725,11 +4660,9 @@
         <v>51</v>
       </c>
       <c r="K47" s="31" t="s">
-        <v>97</v>
-      </c>
-      <c r="L47" s="31" t="s">
-        <v>98</v>
-      </c>
+        <v>91</v>
+      </c>
+      <c r="L47" s="31"/>
       <c r="M47" s="31"/>
       <c r="N47" s="31"/>
       <c r="O47" s="31"/>
@@ -4741,7 +4674,7 @@
       <c r="U47" s="32"/>
       <c r="V47" s="33"/>
       <c r="W47" s="34" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="132" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4752,13 +4685,13 @@
         <v>47</v>
       </c>
       <c r="C48" s="27" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D48" s="27" t="s">
-        <v>149</v>
+        <v>139</v>
       </c>
       <c r="E48" s="35" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="F48" s="29"/>
       <c r="G48" s="30"/>
@@ -4768,11 +4701,9 @@
         <v>51</v>
       </c>
       <c r="K48" s="31" t="s">
-        <v>97</v>
-      </c>
-      <c r="L48" s="31" t="s">
-        <v>151</v>
-      </c>
+        <v>91</v>
+      </c>
+      <c r="L48" s="31"/>
       <c r="M48" s="31"/>
       <c r="N48" s="31"/>
       <c r="O48" s="31"/>
@@ -4784,7 +4715,7 @@
       <c r="U48" s="32"/>
       <c r="V48" s="33"/>
       <c r="W48" s="34" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="123.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4795,13 +4726,13 @@
         <v>47</v>
       </c>
       <c r="C49" s="27" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D49" s="27" t="s">
-        <v>152</v>
+        <v>141</v>
       </c>
       <c r="E49" s="35" t="s">
-        <v>153</v>
+        <v>142</v>
       </c>
       <c r="F49" s="29"/>
       <c r="G49" s="30"/>
@@ -4811,11 +4742,9 @@
         <v>51</v>
       </c>
       <c r="K49" s="31" t="s">
-        <v>97</v>
-      </c>
-      <c r="L49" s="31" t="s">
-        <v>104</v>
-      </c>
+        <v>91</v>
+      </c>
+      <c r="L49" s="31"/>
       <c r="M49" s="31"/>
       <c r="N49" s="31"/>
       <c r="O49" s="31"/>
@@ -4827,7 +4756,7 @@
       <c r="U49" s="32"/>
       <c r="V49" s="33"/>
       <c r="W49" s="34" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="104.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4838,13 +4767,13 @@
         <v>47</v>
       </c>
       <c r="C50" s="27" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D50" s="27" t="s">
-        <v>154</v>
+        <v>143</v>
       </c>
       <c r="E50" s="35" t="s">
-        <v>155</v>
+        <v>144</v>
       </c>
       <c r="F50" s="29"/>
       <c r="G50" s="30"/>
@@ -4854,7 +4783,7 @@
         <v>51</v>
       </c>
       <c r="K50" s="31" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="L50" s="31"/>
       <c r="M50" s="31"/>
@@ -4868,7 +4797,7 @@
       <c r="U50" s="32"/>
       <c r="V50" s="33"/>
       <c r="W50" s="34" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="149.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4879,13 +4808,13 @@
         <v>47</v>
       </c>
       <c r="C51" s="27" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D51" s="27" t="s">
-        <v>156</v>
+        <v>145</v>
       </c>
       <c r="E51" s="35" t="s">
-        <v>157</v>
+        <v>146</v>
       </c>
       <c r="F51" s="29"/>
       <c r="G51" s="30"/>
@@ -4895,11 +4824,9 @@
         <v>51</v>
       </c>
       <c r="K51" s="31" t="s">
-        <v>97</v>
-      </c>
-      <c r="L51" s="31" t="s">
-        <v>151</v>
-      </c>
+        <v>91</v>
+      </c>
+      <c r="L51" s="31"/>
       <c r="M51" s="31"/>
       <c r="N51" s="31"/>
       <c r="O51" s="31"/>
@@ -4911,7 +4838,7 @@
       <c r="U51" s="32"/>
       <c r="V51" s="33"/>
       <c r="W51" s="34" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="134.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4922,13 +4849,13 @@
         <v>47</v>
       </c>
       <c r="C52" s="27" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D52" s="27" t="s">
-        <v>158</v>
+        <v>147</v>
       </c>
       <c r="E52" s="35" t="s">
-        <v>159</v>
+        <v>148</v>
       </c>
       <c r="F52" s="29"/>
       <c r="G52" s="30"/>
@@ -4938,7 +4865,7 @@
         <v>51</v>
       </c>
       <c r="K52" s="31" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="L52" s="31"/>
       <c r="M52" s="31"/>
@@ -4952,7 +4879,7 @@
       <c r="U52" s="32"/>
       <c r="V52" s="33"/>
       <c r="W52" s="34" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="161.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4963,13 +4890,13 @@
         <v>47</v>
       </c>
       <c r="C53" s="27" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D53" s="27" t="s">
-        <v>160</v>
+        <v>149</v>
       </c>
       <c r="E53" s="35" t="s">
-        <v>161</v>
+        <v>150</v>
       </c>
       <c r="F53" s="29"/>
       <c r="G53" s="30"/>
@@ -4979,7 +4906,7 @@
         <v>51</v>
       </c>
       <c r="K53" s="31" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="L53" s="31"/>
       <c r="M53" s="31"/>
@@ -4993,7 +4920,7 @@
       <c r="U53" s="32"/>
       <c r="V53" s="33"/>
       <c r="W53" s="34" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="137.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5004,13 +4931,13 @@
         <v>47</v>
       </c>
       <c r="C54" s="27" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D54" s="27" t="s">
-        <v>162</v>
+        <v>151</v>
       </c>
       <c r="E54" s="35" t="s">
-        <v>163</v>
+        <v>152</v>
       </c>
       <c r="F54" s="29"/>
       <c r="G54" s="30"/>
@@ -5020,7 +4947,7 @@
         <v>51</v>
       </c>
       <c r="K54" s="31" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="L54" s="31"/>
       <c r="M54" s="31"/>
@@ -5034,7 +4961,7 @@
       <c r="U54" s="32"/>
       <c r="V54" s="33"/>
       <c r="W54" s="34" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="149.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5045,13 +4972,13 @@
         <v>47</v>
       </c>
       <c r="C55" s="27" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D55" s="27" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="E55" s="35" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="F55" s="29"/>
       <c r="G55" s="30"/>
@@ -5061,7 +4988,7 @@
         <v>51</v>
       </c>
       <c r="K55" s="31" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="L55" s="31"/>
       <c r="M55" s="31"/>
@@ -5075,7 +5002,7 @@
       <c r="U55" s="32"/>
       <c r="V55" s="33"/>
       <c r="W55" s="34" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="129.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5086,13 +5013,13 @@
         <v>47</v>
       </c>
       <c r="C56" s="27" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D56" s="27" t="s">
-        <v>166</v>
+        <v>155</v>
       </c>
       <c r="E56" s="35" t="s">
-        <v>167</v>
+        <v>156</v>
       </c>
       <c r="F56" s="29"/>
       <c r="G56" s="30"/>
@@ -5102,7 +5029,7 @@
         <v>51</v>
       </c>
       <c r="K56" s="31" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="L56" s="31"/>
       <c r="M56" s="31"/>
@@ -5116,7 +5043,7 @@
       <c r="U56" s="32"/>
       <c r="V56" s="33"/>
       <c r="W56" s="34" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="135.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5127,13 +5054,13 @@
         <v>47</v>
       </c>
       <c r="C57" s="27" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D57" s="27" t="s">
-        <v>168</v>
+        <v>157</v>
       </c>
       <c r="E57" s="35" t="s">
-        <v>169</v>
+        <v>158</v>
       </c>
       <c r="F57" s="29"/>
       <c r="G57" s="30"/>
@@ -5157,7 +5084,7 @@
       <c r="U57" s="32"/>
       <c r="V57" s="33"/>
       <c r="W57" s="34" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="145.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5168,28 +5095,28 @@
         <v>47</v>
       </c>
       <c r="C58" s="27" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D58" s="27" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
       <c r="E58" s="35" t="s">
-        <v>171</v>
+        <v>160</v>
       </c>
       <c r="F58" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="G58" s="30" t="s">
+        <v>161</v>
+      </c>
+      <c r="H58" s="30" t="s">
+        <v>162</v>
+      </c>
+      <c r="I58" s="30" t="s">
+        <v>163</v>
+      </c>
+      <c r="J58" s="31" t="s">
         <v>63</v>
-      </c>
-      <c r="G58" s="30" t="s">
-        <v>172</v>
-      </c>
-      <c r="H58" s="30" t="s">
-        <v>173</v>
-      </c>
-      <c r="I58" s="30" t="s">
-        <v>174</v>
-      </c>
-      <c r="J58" s="31" t="s">
-        <v>65</v>
       </c>
       <c r="K58" s="31"/>
       <c r="L58" s="31"/>
@@ -5204,7 +5131,7 @@
       <c r="U58" s="32"/>
       <c r="V58" s="33"/>
       <c r="W58" s="36" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="132.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5218,25 +5145,25 @@
         <v>48</v>
       </c>
       <c r="D59" s="38" t="s">
-        <v>175</v>
+        <v>164</v>
       </c>
       <c r="E59" s="39" t="s">
-        <v>176</v>
+        <v>165</v>
       </c>
       <c r="F59" s="40" t="s">
+        <v>61</v>
+      </c>
+      <c r="G59" s="41" t="s">
+        <v>166</v>
+      </c>
+      <c r="H59" s="41" t="s">
+        <v>167</v>
+      </c>
+      <c r="I59" s="41" t="s">
+        <v>168</v>
+      </c>
+      <c r="J59" s="42" t="s">
         <v>63</v>
-      </c>
-      <c r="G59" s="41" t="s">
-        <v>177</v>
-      </c>
-      <c r="H59" s="41" t="s">
-        <v>178</v>
-      </c>
-      <c r="I59" s="41" t="s">
-        <v>179</v>
-      </c>
-      <c r="J59" s="42" t="s">
-        <v>65</v>
       </c>
       <c r="K59" s="42"/>
       <c r="L59" s="42"/>
@@ -5251,7 +5178,7 @@
       <c r="U59" s="43"/>
       <c r="V59" s="44"/>
       <c r="W59" s="36" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="128.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5265,10 +5192,10 @@
         <v>48</v>
       </c>
       <c r="D60" s="46" t="s">
-        <v>180</v>
+        <v>169</v>
       </c>
       <c r="E60" s="47" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="F60" s="48"/>
       <c r="G60" s="49"/>
@@ -5278,7 +5205,7 @@
         <v>51</v>
       </c>
       <c r="K60" s="50" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="L60" s="50"/>
       <c r="M60" s="50"/>
@@ -5292,7 +5219,7 @@
       <c r="U60" s="51"/>
       <c r="V60" s="52"/>
       <c r="W60" s="53" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10095,7 +10022,7 @@
   </sheetPr>
   <dimension ref="A1:A8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="39" zoomScaleNormal="39" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="I15" activeCellId="0" sqref="I15"/>
     </sheetView>
   </sheetViews>
@@ -10103,17 +10030,17 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10123,22 +10050,22 @@
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -10159,13 +10086,13 @@
   </sheetPr>
   <dimension ref="A1:G960"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="39" zoomScaleNormal="39" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.46484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.47265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.82"/>
@@ -10178,50 +10105,50 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="17" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="B1" s="17" t="s">
         <v>25</v>
       </c>
       <c r="C1" s="17" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="D1" s="17" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
       <c r="F1" s="54" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
       <c r="G1" s="55" t="s">
-        <v>188</v>
+        <v>177</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="56" t="s">
-        <v>189</v>
+        <v>178</v>
       </c>
       <c r="B2" s="56" t="s">
-        <v>190</v>
+        <v>179</v>
       </c>
       <c r="C2" s="57" t="s">
-        <v>191</v>
+        <v>180</v>
       </c>
       <c r="D2" s="57" t="s">
-        <v>192</v>
+        <v>181</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="56" t="s">
-        <v>193</v>
+        <v>182</v>
       </c>
       <c r="B3" s="56" t="s">
-        <v>190</v>
+        <v>179</v>
       </c>
       <c r="C3" s="57" t="s">
-        <v>194</v>
+        <v>183</v>
       </c>
       <c r="D3" s="57" t="s">
-        <v>195</v>
+        <v>184</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10229,111 +10156,111 @@
         <v>48</v>
       </c>
       <c r="B4" s="56" t="s">
-        <v>190</v>
+        <v>179</v>
       </c>
       <c r="C4" s="57" t="n">
         <v>446.447</v>
       </c>
       <c r="D4" s="58" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="56" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
       <c r="B5" s="56" t="s">
-        <v>190</v>
+        <v>179</v>
       </c>
       <c r="C5" s="57" t="s">
-        <v>198</v>
+        <v>187</v>
       </c>
       <c r="D5" s="57" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="56" t="s">
-        <v>200</v>
+        <v>189</v>
       </c>
       <c r="B6" s="56" t="s">
+        <v>179</v>
+      </c>
+      <c r="C6" s="57" t="s">
         <v>190</v>
       </c>
-      <c r="C6" s="57" t="s">
-        <v>201</v>
-      </c>
       <c r="D6" s="58" t="s">
-        <v>202</v>
+        <v>191</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="56" t="s">
-        <v>203</v>
+        <v>192</v>
       </c>
       <c r="B7" s="56" t="s">
-        <v>190</v>
+        <v>179</v>
       </c>
       <c r="C7" s="57" t="s">
-        <v>204</v>
+        <v>193</v>
       </c>
       <c r="D7" s="58" t="s">
-        <v>205</v>
+        <v>194</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="56" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B8" s="56" t="s">
-        <v>190</v>
+        <v>179</v>
       </c>
       <c r="C8" s="57" t="s">
-        <v>206</v>
+        <v>195</v>
       </c>
       <c r="D8" s="58" t="s">
-        <v>207</v>
+        <v>196</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="56" t="s">
-        <v>208</v>
+        <v>197</v>
       </c>
       <c r="B9" s="56" t="s">
-        <v>190</v>
+        <v>179</v>
       </c>
       <c r="C9" s="57" t="s">
-        <v>209</v>
+        <v>198</v>
       </c>
       <c r="D9" s="58" t="s">
-        <v>210</v>
+        <v>199</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="43.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="56" t="s">
-        <v>211</v>
+        <v>200</v>
       </c>
       <c r="B10" s="56" t="s">
-        <v>190</v>
+        <v>179</v>
       </c>
       <c r="C10" s="58" t="s">
-        <v>212</v>
+        <v>201</v>
       </c>
       <c r="D10" s="57" t="s">
-        <v>213</v>
+        <v>202</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="56" t="s">
-        <v>214</v>
+        <v>203</v>
       </c>
       <c r="B11" s="56" t="s">
-        <v>190</v>
+        <v>179</v>
       </c>
       <c r="C11" s="57" t="s">
-        <v>215</v>
+        <v>204</v>
       </c>
       <c r="D11" s="58" t="s">
-        <v>216</v>
+        <v>205</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -11305,11 +11232,11 @@
   </sheetPr>
   <dimension ref="A1:B1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="39" zoomScaleNormal="39" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.46484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.47265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.17"/>
@@ -11326,15 +11253,15 @@
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="59" t="s">
-        <v>217</v>
+        <v>206</v>
       </c>
       <c r="B2" s="59" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="59" t="s">
-        <v>218</v>
+        <v>207</v>
       </c>
       <c r="B3" s="59" t="s">
         <v>51</v>

</xml_diff>